<commit_message>
Refactor photo upload handling in GraveForm and GravesImportParser to dynamically generate storage paths based on cemetery commune
</commit_message>
<xml_diff>
--- a/public/template/TemplateLietSy.xlsx
+++ b/public/template/TemplateLietSy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BT\Website\Project_Laravel\quanlynghiadia\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF7357-3EDB-4DF2-B3FE-E0094A62CBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BCBCAA-DA63-4DC4-A788-37B6C8C85EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70627EA3-9096-4FDB-85C6-025EED12D626}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Họ và tên
 Liệt sỹ</t>
@@ -77,6 +77,34 @@
   </si>
   <si>
     <t xml:space="preserve">   Lô     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đỗ Văn Cừ </t>
+  </si>
+  <si>
+    <t>Trung đội phó</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trung đội trưởng
+</t>
+  </si>
+  <si>
+    <t>18-6-1969</t>
+  </si>
+  <si>
+    <t>ZB 164b</t>
+  </si>
+  <si>
+    <t>135TTga/04-04-1957</t>
+  </si>
+  <si>
+    <t>Anh ruột</t>
+  </si>
+  <si>
+    <t>Lê Hồng Quân</t>
+  </si>
+  <si>
+    <t>1762188222-3f8776.png</t>
   </si>
 </sst>
 </file>
@@ -146,17 +174,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EA79F6-3883-4F31-B78B-F992570F2595}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,68 +539,100 @@
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>1928</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Refactor grave details and database schema
- Updated grave-detail view to remove unnecessary fields and display new fields: hometown, enlistment date, rank, and unit.
- Modified search view to reflect changes in displaying birth date and rank/unit information.
- Created migration to add new fields (hometown, enlistment_date, rank, unit) to graves table and migrate existing data from rank_and_unit.
- Added migration to remove unnecessary fields from graves table, streamlining the database structure.
</commit_message>
<xml_diff>
--- a/public/template/TemplateLietSy.xlsx
+++ b/public/template/TemplateLietSy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BT\Website\Project_Laravel\quanlynghiadia\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BCBCAA-DA63-4DC4-A788-37B6C8C85EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7010918F-3416-40FB-830C-912248C34464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70627EA3-9096-4FDB-85C6-025EED12D626}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A25D3AF0-438D-4E06-8D09-BFA45B07CD4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,82 +36,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Họ và tên
-Liệt sỹ</t>
-  </si>
-  <si>
-    <t>Năm sinh</t>
-  </si>
-  <si>
-    <t>Cấp bậc, chức vụ, đơn vị</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Nguyên Quán</t>
+  </si>
+  <si>
+    <t>Ngày tháng
+năm sinh</t>
+  </si>
+  <si>
+    <t>Ngày tháng
+năm nhập ngũ</t>
+  </si>
+  <si>
+    <t>Ngày tháng
+năm Hy sinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cấp bậc </t>
   </si>
   <si>
     <t>Chức vụ</t>
   </si>
   <si>
-    <t>Ngày tháng năm hy sinh</t>
-  </si>
-  <si>
-    <t>Số bằng TQGC</t>
-  </si>
-  <si>
-    <t>Số QĐ, ngày, tháng, năm cấp</t>
-  </si>
-  <si>
-    <t>Quan hệ 
-với liệt sỹ</t>
-  </si>
-  <si>
-    <t>Thân nhân</t>
-  </si>
-  <si>
-    <t>Ghi chú</t>
-  </si>
-  <si>
-    <t>Ảnh liệt sỹ</t>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>Nguyễn Hữu Trường</t>
+  </si>
+  <si>
+    <t>Thôn 2 - Xã Lý Nhân</t>
+  </si>
+  <si>
+    <t>13/02/1952</t>
+  </si>
+  <si>
+    <t>17/03/1954</t>
+  </si>
+  <si>
+    <t>Chiến sỹ</t>
+  </si>
+  <si>
+    <t>F320</t>
+  </si>
+  <si>
+    <t>Lô</t>
+  </si>
+  <si>
+    <t>Ảnh liệt sĩ</t>
   </si>
   <si>
     <t>Ảnh mộ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Lô     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đỗ Văn Cừ </t>
-  </si>
-  <si>
-    <t>Trung đội phó</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trung đội trưởng
-</t>
-  </si>
-  <si>
-    <t>18-6-1969</t>
-  </si>
-  <si>
-    <t>ZB 164b</t>
-  </si>
-  <si>
-    <t>135TTga/04-04-1957</t>
-  </si>
-  <si>
-    <t>Anh ruột</t>
-  </si>
-  <si>
-    <t>Lê Hồng Quân</t>
-  </si>
-  <si>
-    <t>1762188222-3f8776.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,22 +109,39 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,23 +175,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,135 +557,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EA79F6-3883-4F31-B78B-F992570F2595}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593CACB8-AD3E-4D8F-8C53-CC573F9E8A65}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" style="5" customWidth="1"/>
+    <col min="5" max="6" width="23.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="21" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>1928</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="I3" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="E1:E2"/>
+  <mergeCells count="12">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor GravesTable and GravesImportParser for improved data handling and UI consistency
</commit_message>
<xml_diff>
--- a/public/template/TemplateLietSy.xlsx
+++ b/public/template/TemplateLietSy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7010918F-3416-40FB-830C-912248C34464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8446F1DD-21B3-46DB-81FA-F90199A04720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A25D3AF0-438D-4E06-8D09-BFA45B07CD4A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>STT</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Ảnh mộ</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -188,12 +191,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -203,26 +240,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,119 +583,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593CACB8-AD3E-4D8F-8C53-CC573F9E8A65}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" style="5" customWidth="1"/>
-    <col min="5" max="6" width="23.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="21" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="23.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.77734375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="J3" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>